<commit_message>
saving lej data after review; no changes
</commit_message>
<xml_diff>
--- a/data/input/SY2016-2021 collected fish with tag_lej.xlsx
+++ b/data/input/SY2016-2021 collected fish with tag_lej.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurajenkins/Desktop/Kelting rate analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverKelt\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55A130F-D3F0-1043-8EBE-2751BD58CC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C21D316-2DDD-4D64-8F6D-F40A8EE85606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39480" yWindow="580" windowWidth="35120" windowHeight="19780" activeTab="2" xr2:uid="{6091E659-C70E-2D41-AE04-6C1C29E40EA9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6091E659-C70E-2D41-AE04-6C1C29E40EA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -3017,7 +3017,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -5152,7 +5152,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F01B6109-5307-9C45-A9D9-6395CDD19F44}" name="Table11" displayName="Table11" ref="A1:AU161" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96" dataCellStyle="Normal 2 3">
-  <autoFilter ref="A1:AU161" xr:uid="{F01B6109-5307-9C45-A9D9-6395CDD19F44}"/>
   <tableColumns count="47">
     <tableColumn id="1" xr3:uid="{2992E537-AFFD-404A-9040-A23B3573C567}" name="Sequence" dataDxfId="95" dataCellStyle="Normal 2 3"/>
     <tableColumn id="2" xr3:uid="{D44A95E0-C342-7241-9750-D20AD05F7501}" name="Activity Date" dataDxfId="94" dataCellStyle="Normal 2 3"/>
@@ -5208,7 +5207,6 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{57E43195-35A4-EE41-8593-96DFCD134AD5}" name="Table10" displayName="Table10" ref="A1:AU221" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
-  <autoFilter ref="A1:AU221" xr:uid="{57E43195-35A4-EE41-8593-96DFCD134AD5}"/>
   <tableColumns count="47">
     <tableColumn id="1" xr3:uid="{AD6348A3-0E4B-1E44-9ABE-F8E65A24B760}" name="Sequence" dataDxfId="46"/>
     <tableColumn id="2" xr3:uid="{56686C2F-F838-BE4F-B97E-3F21C711758E}" name="Activity Date" dataDxfId="45"/>
@@ -5263,9 +5261,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5303,7 +5301,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5409,7 +5407,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5551,7 +5549,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5561,24 +5559,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2EDE034-D56F-8D47-ABF2-A8A07729FBB5}">
   <dimension ref="C2:E9"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E9"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="18"/>
   <cols>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.58203125" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5">
       <c r="D2" s="22" t="s">
         <v>988</v>
       </c>
       <c r="E2" s="22"/>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:5">
       <c r="D3" t="s">
         <v>990</v>
       </c>
@@ -5586,7 +5584,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5">
       <c r="C4">
         <v>2016</v>
       </c>
@@ -5597,7 +5595,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5">
       <c r="C5">
         <v>2017</v>
       </c>
@@ -5608,7 +5606,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:5">
       <c r="C6">
         <v>2018</v>
       </c>
@@ -5619,7 +5617,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:5">
       <c r="C7">
         <v>2019</v>
       </c>
@@ -5630,7 +5628,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5">
       <c r="C8">
         <v>2020</v>
       </c>
@@ -5641,7 +5639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5">
       <c r="C9">
         <v>2021</v>
       </c>
@@ -5664,49 +5662,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C603D3F7-1324-3A4A-8D54-36B833AC1A12}">
   <dimension ref="A1:AU161"/>
   <sheetViews>
-    <sheetView topLeftCell="AC126" workbookViewId="0">
-      <selection activeCell="AU134" sqref="AU134"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="18"/>
   <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.25" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.75" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.58203125" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.4140625" customWidth="1"/>
+    <col min="12" max="12" width="18.4140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
     <col min="15" max="15" width="22" style="7" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" customWidth="1"/>
-    <col min="18" max="18" width="24.140625" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" customWidth="1"/>
+    <col min="17" max="17" width="14.4140625" customWidth="1"/>
+    <col min="18" max="18" width="24.1640625" customWidth="1"/>
     <col min="19" max="19" width="23" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" customWidth="1"/>
-    <col min="25" max="26" width="11.7109375" customWidth="1"/>
+    <col min="23" max="23" width="11.83203125" customWidth="1"/>
+    <col min="25" max="26" width="11.75" customWidth="1"/>
     <col min="28" max="28" width="15" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" customWidth="1"/>
-    <col min="31" max="31" width="13.140625" customWidth="1"/>
+    <col min="30" max="30" width="10.83203125" customWidth="1"/>
+    <col min="31" max="31" width="13.1640625" customWidth="1"/>
     <col min="32" max="32" width="20" customWidth="1"/>
-    <col min="36" max="36" width="10.85546875" customWidth="1"/>
-    <col min="37" max="37" width="14.5703125" customWidth="1"/>
+    <col min="36" max="36" width="10.83203125" customWidth="1"/>
+    <col min="37" max="37" width="14.58203125" customWidth="1"/>
     <col min="38" max="38" width="17" customWidth="1"/>
-    <col min="39" max="39" width="13.42578125" customWidth="1"/>
-    <col min="40" max="40" width="12.42578125" customWidth="1"/>
-    <col min="41" max="41" width="17.28515625" customWidth="1"/>
-    <col min="42" max="42" width="13.5703125" customWidth="1"/>
-    <col min="43" max="43" width="16.5703125" customWidth="1"/>
-    <col min="44" max="44" width="11.7109375" customWidth="1"/>
-    <col min="45" max="45" width="14.42578125" customWidth="1"/>
-    <col min="46" max="46" width="15.85546875" customWidth="1"/>
-    <col min="47" max="47" width="10.85546875" customWidth="1"/>
+    <col min="39" max="39" width="13.4140625" customWidth="1"/>
+    <col min="40" max="40" width="12.4140625" customWidth="1"/>
+    <col min="41" max="41" width="17.25" customWidth="1"/>
+    <col min="42" max="42" width="13.58203125" customWidth="1"/>
+    <col min="43" max="43" width="16.58203125" customWidth="1"/>
+    <col min="44" max="44" width="11.75" customWidth="1"/>
+    <col min="45" max="45" width="14.4140625" customWidth="1"/>
+    <col min="46" max="46" width="15.83203125" customWidth="1"/>
+    <col min="47" max="47" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -5849,7 +5847,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47">
       <c r="A2" s="11">
         <v>1979</v>
       </c>
@@ -5962,7 +5960,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47">
       <c r="A3" s="11">
         <v>871</v>
       </c>
@@ -6073,7 +6071,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47">
       <c r="A4" s="11">
         <v>3665</v>
       </c>
@@ -6184,7 +6182,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47">
       <c r="A5" s="11">
         <v>3312</v>
       </c>
@@ -6295,7 +6293,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47">
       <c r="A6" s="11">
         <v>1437</v>
       </c>
@@ -6406,7 +6404,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47">
       <c r="A7" s="11">
         <v>1455</v>
       </c>
@@ -6515,7 +6513,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47">
       <c r="A8" s="11">
         <v>53</v>
       </c>
@@ -6626,7 +6624,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47">
       <c r="A9" s="11">
         <v>3073</v>
       </c>
@@ -6735,7 +6733,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47">
       <c r="A10" s="11">
         <v>2002</v>
       </c>
@@ -6846,7 +6844,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47">
       <c r="A11" s="11">
         <v>1903</v>
       </c>
@@ -6957,7 +6955,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47">
       <c r="A12" s="11">
         <v>1540</v>
       </c>
@@ -7068,7 +7066,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47">
       <c r="A13" s="11">
         <v>1354</v>
       </c>
@@ -7179,7 +7177,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47">
       <c r="A14" s="11">
         <v>1424</v>
       </c>
@@ -7288,7 +7286,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47">
       <c r="A15" s="11">
         <v>3235</v>
       </c>
@@ -7399,7 +7397,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" s="1" customFormat="1">
       <c r="A16" s="15">
         <v>530</v>
       </c>
@@ -7542,7 +7540,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" s="1" customFormat="1">
       <c r="A17" s="15">
         <v>2587</v>
       </c>
@@ -7685,7 +7683,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" s="1" customFormat="1">
       <c r="A18" s="15">
         <v>3412</v>
       </c>
@@ -7828,7 +7826,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" s="1" customFormat="1">
       <c r="A19" s="15">
         <v>694</v>
       </c>
@@ -7971,7 +7969,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" s="1" customFormat="1">
       <c r="A20" s="15">
         <v>961</v>
       </c>
@@ -8114,7 +8112,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" s="1" customFormat="1">
       <c r="A21" s="15">
         <v>3397</v>
       </c>
@@ -8257,7 +8255,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" s="1" customFormat="1">
       <c r="A22" s="15">
         <v>2370</v>
       </c>
@@ -8400,7 +8398,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" s="1" customFormat="1">
       <c r="A23" s="15">
         <v>2249</v>
       </c>
@@ -8543,7 +8541,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" s="1" customFormat="1">
       <c r="A24" s="15">
         <v>2364</v>
       </c>
@@ -8686,7 +8684,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" s="1" customFormat="1">
       <c r="A25" s="15">
         <v>2604</v>
       </c>
@@ -8829,7 +8827,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" s="1" customFormat="1">
       <c r="A26" s="15">
         <v>3211</v>
       </c>
@@ -8972,7 +8970,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" s="1" customFormat="1">
       <c r="A27" s="15">
         <v>225</v>
       </c>
@@ -9115,7 +9113,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" s="1" customFormat="1">
       <c r="A28" s="15">
         <v>227</v>
       </c>
@@ -9258,7 +9256,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" s="1" customFormat="1">
       <c r="A29" s="15">
         <v>810</v>
       </c>
@@ -9401,7 +9399,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" s="1" customFormat="1">
       <c r="A30" s="15">
         <v>3618</v>
       </c>
@@ -9544,7 +9542,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" s="1" customFormat="1">
       <c r="A31" s="15">
         <v>1076</v>
       </c>
@@ -9687,7 +9685,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" s="1" customFormat="1">
       <c r="A32" s="15">
         <v>4355</v>
       </c>
@@ -9830,7 +9828,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" s="1" customFormat="1">
       <c r="A33" s="15">
         <v>4201</v>
       </c>
@@ -9973,7 +9971,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" s="1" customFormat="1">
       <c r="A34" s="15">
         <v>190</v>
       </c>
@@ -10116,7 +10114,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" s="1" customFormat="1">
       <c r="A35" s="15">
         <v>3814</v>
       </c>
@@ -10259,7 +10257,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" s="1" customFormat="1">
       <c r="A36" s="15">
         <v>651</v>
       </c>
@@ -10402,7 +10400,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" s="1" customFormat="1">
       <c r="A37" s="15">
         <v>3342</v>
       </c>
@@ -10545,7 +10543,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" s="1" customFormat="1">
       <c r="A38" s="15">
         <v>3351</v>
       </c>
@@ -10688,7 +10686,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:47" s="1" customFormat="1">
       <c r="A39" s="15">
         <v>650</v>
       </c>
@@ -10831,7 +10829,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" s="1" customFormat="1">
       <c r="A40" s="15">
         <v>2765</v>
       </c>
@@ -10974,7 +10972,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" s="1" customFormat="1">
       <c r="A41" s="15">
         <v>967</v>
       </c>
@@ -11117,7 +11115,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" s="1" customFormat="1">
       <c r="A42" s="15">
         <v>2589</v>
       </c>
@@ -11260,7 +11258,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" s="1" customFormat="1">
       <c r="A43" s="15">
         <v>1090</v>
       </c>
@@ -11403,7 +11401,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" s="1" customFormat="1">
       <c r="A44" s="15">
         <v>739</v>
       </c>
@@ -11546,7 +11544,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" s="1" customFormat="1">
       <c r="A45" s="15">
         <v>4029</v>
       </c>
@@ -11689,7 +11687,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:47" s="1" customFormat="1">
       <c r="A46" s="15">
         <v>2737</v>
       </c>
@@ -11832,7 +11830,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:47" s="1" customFormat="1">
       <c r="A47" s="15">
         <v>3848</v>
       </c>
@@ -11975,7 +11973,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" s="1" customFormat="1">
       <c r="A48" s="15">
         <v>2541</v>
       </c>
@@ -12118,7 +12116,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:47" s="1" customFormat="1">
       <c r="A49" s="15">
         <v>2246</v>
       </c>
@@ -12261,7 +12259,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:47" s="1" customFormat="1">
       <c r="A50" s="15">
         <v>3833</v>
       </c>
@@ -12404,7 +12402,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:47" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:47" s="21" customFormat="1" ht="15.6">
       <c r="K51" s="21" t="s">
         <v>321</v>
       </c>
@@ -12412,7 +12410,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="52" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:47" s="5" customFormat="1">
       <c r="A52" s="14">
         <v>511</v>
       </c>
@@ -12555,7 +12553,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:47" s="5" customFormat="1">
       <c r="A53" s="14">
         <v>3122</v>
       </c>
@@ -12698,7 +12696,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:47" s="5" customFormat="1">
       <c r="A54" s="14">
         <v>985</v>
       </c>
@@ -12841,7 +12839,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:47" s="5" customFormat="1">
       <c r="A55" s="14">
         <v>3577</v>
       </c>
@@ -12984,7 +12982,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:47" s="5" customFormat="1">
       <c r="A56" s="14">
         <v>4297</v>
       </c>
@@ -13127,7 +13125,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:47" s="5" customFormat="1">
       <c r="A57" s="14">
         <v>2178</v>
       </c>
@@ -13270,7 +13268,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:47" s="5" customFormat="1">
       <c r="A58" s="14">
         <v>162</v>
       </c>
@@ -13413,7 +13411,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:47" s="5" customFormat="1">
       <c r="A59" s="14">
         <v>982</v>
       </c>
@@ -13556,7 +13554,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:47" s="5" customFormat="1">
       <c r="A60" s="14">
         <v>4293</v>
       </c>
@@ -13699,7 +13697,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:47" s="5" customFormat="1">
       <c r="A61" s="14">
         <v>3141</v>
       </c>
@@ -13842,7 +13840,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:47" s="5" customFormat="1">
       <c r="A62" s="14">
         <v>2319</v>
       </c>
@@ -13985,7 +13983,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:47" s="5" customFormat="1">
       <c r="A63" s="14">
         <v>3119</v>
       </c>
@@ -14128,7 +14126,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:47" s="5" customFormat="1">
       <c r="A64" s="14">
         <v>989</v>
       </c>
@@ -14271,7 +14269,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" s="5" customFormat="1">
       <c r="A65" s="14">
         <v>387</v>
       </c>
@@ -14414,7 +14412,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" s="5" customFormat="1">
       <c r="A66" s="14">
         <v>3574</v>
       </c>
@@ -14557,7 +14555,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" s="5" customFormat="1">
       <c r="A67" s="14">
         <v>2429</v>
       </c>
@@ -14700,7 +14698,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" s="5" customFormat="1">
       <c r="A68" s="14">
         <v>2698</v>
       </c>
@@ -14843,7 +14841,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" s="5" customFormat="1">
       <c r="A69" s="14">
         <v>1847</v>
       </c>
@@ -14986,7 +14984,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" s="5" customFormat="1">
       <c r="A70" s="14">
         <v>4160</v>
       </c>
@@ -15129,7 +15127,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" s="5" customFormat="1">
       <c r="A71" s="14">
         <v>940</v>
       </c>
@@ -15272,7 +15270,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:47" s="5" customFormat="1">
       <c r="A72" s="14">
         <v>4045</v>
       </c>
@@ -15415,7 +15413,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:47" s="5" customFormat="1">
       <c r="A73" s="14">
         <v>991</v>
       </c>
@@ -15558,7 +15556,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:47" s="5" customFormat="1">
       <c r="A74" s="14">
         <v>3135</v>
       </c>
@@ -15701,7 +15699,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:47" s="5" customFormat="1">
       <c r="A75" s="14">
         <v>2972</v>
       </c>
@@ -15844,7 +15842,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:47" s="5" customFormat="1">
       <c r="A76" s="14">
         <v>786</v>
       </c>
@@ -15987,7 +15985,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:47" s="5" customFormat="1">
       <c r="A77" s="14">
         <v>4290</v>
       </c>
@@ -16130,7 +16128,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:47" s="5" customFormat="1">
       <c r="A78" s="14">
         <v>2390</v>
       </c>
@@ -16273,7 +16271,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:47" s="5" customFormat="1">
       <c r="A79" s="14">
         <v>3130</v>
       </c>
@@ -16416,7 +16414,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="80" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:47" s="5" customFormat="1">
       <c r="A80" s="14">
         <v>479</v>
       </c>
@@ -16559,7 +16557,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:47" s="5" customFormat="1">
       <c r="A81" s="14">
         <v>267</v>
       </c>
@@ -16702,7 +16700,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="82" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:47" s="5" customFormat="1">
       <c r="A82" s="14">
         <v>462</v>
       </c>
@@ -16845,7 +16843,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:47" s="5" customFormat="1">
       <c r="A83" s="14">
         <v>2427</v>
       </c>
@@ -16988,7 +16986,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:47" s="5" customFormat="1">
       <c r="A84" s="14">
         <v>3441</v>
       </c>
@@ -17131,7 +17129,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="85" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:47" s="5" customFormat="1">
       <c r="A85" s="14">
         <v>2384</v>
       </c>
@@ -17274,7 +17272,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="86" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:47" s="5" customFormat="1">
       <c r="A86" s="14">
         <v>1391</v>
       </c>
@@ -17417,7 +17415,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:47" s="5" customFormat="1">
       <c r="A87" s="14">
         <v>2644</v>
       </c>
@@ -17560,7 +17558,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="88" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:47" s="5" customFormat="1">
       <c r="A88" s="14">
         <v>151</v>
       </c>
@@ -17703,7 +17701,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="89" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:47" s="5" customFormat="1">
       <c r="A89" s="14">
         <v>2235</v>
       </c>
@@ -17846,7 +17844,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="90" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:47" s="5" customFormat="1">
       <c r="A90" s="14">
         <v>4292</v>
       </c>
@@ -17989,7 +17987,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="91" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:47" s="5" customFormat="1">
       <c r="A91" s="14">
         <v>2658</v>
       </c>
@@ -18132,7 +18130,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:47" s="5" customFormat="1">
       <c r="A92" s="14">
         <v>3429</v>
       </c>
@@ -18275,7 +18273,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="93" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:47" s="5" customFormat="1">
       <c r="A93" s="14">
         <v>477</v>
       </c>
@@ -18418,7 +18416,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:47" s="5" customFormat="1">
       <c r="A94" s="14">
         <v>4038</v>
       </c>
@@ -18561,7 +18559,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="95" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:47" s="1" customFormat="1">
       <c r="A95" s="17">
         <v>5714</v>
       </c>
@@ -18704,7 +18702,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="96" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:47" s="1" customFormat="1">
       <c r="A96" s="17">
         <v>4880</v>
       </c>
@@ -18847,7 +18845,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="97" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:47" s="1" customFormat="1">
       <c r="A97" s="17">
         <v>5410</v>
       </c>
@@ -18990,7 +18988,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="98" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:47" s="1" customFormat="1">
       <c r="A98" s="17">
         <v>4877</v>
       </c>
@@ -19133,7 +19131,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="99" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:47" s="1" customFormat="1">
       <c r="A99" s="17">
         <v>4702</v>
       </c>
@@ -19276,7 +19274,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="100" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:47" s="1" customFormat="1">
       <c r="A100" s="17">
         <v>5363</v>
       </c>
@@ -19419,7 +19417,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="101" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:47" s="1" customFormat="1">
       <c r="A101" s="17">
         <v>5261</v>
       </c>
@@ -19562,7 +19560,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="102" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:47" s="1" customFormat="1">
       <c r="A102" s="17">
         <v>5039</v>
       </c>
@@ -19705,7 +19703,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="103" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:47" s="1" customFormat="1">
       <c r="A103" s="17">
         <v>5411</v>
       </c>
@@ -19848,7 +19846,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="104" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:47" s="1" customFormat="1">
       <c r="A104" s="17">
         <v>5025</v>
       </c>
@@ -19991,7 +19989,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="105" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:47" s="1" customFormat="1">
       <c r="A105" s="17">
         <v>5495</v>
       </c>
@@ -20134,7 +20132,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="106" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:47" s="1" customFormat="1">
       <c r="A106" s="17">
         <v>5335</v>
       </c>
@@ -20277,7 +20275,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="107" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:47" s="1" customFormat="1">
       <c r="A107" s="17">
         <v>4401</v>
       </c>
@@ -20420,7 +20418,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="108" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:47" s="1" customFormat="1">
       <c r="A108" s="17">
         <v>4827</v>
       </c>
@@ -20563,7 +20561,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="109" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:47" s="1" customFormat="1">
       <c r="A109" s="17">
         <v>4851</v>
       </c>
@@ -20706,7 +20704,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="110" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:47" s="1" customFormat="1">
       <c r="A110" s="17">
         <v>4589</v>
       </c>
@@ -20849,7 +20847,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="111" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:47" s="1" customFormat="1">
       <c r="A111" s="17">
         <v>5317</v>
       </c>
@@ -20992,7 +20990,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="112" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:47" s="1" customFormat="1">
       <c r="A112" s="17">
         <v>5286</v>
       </c>
@@ -21135,7 +21133,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="113" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:47" s="1" customFormat="1">
       <c r="A113" s="17">
         <v>4565</v>
       </c>
@@ -21278,7 +21276,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="114" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:47" s="1" customFormat="1">
       <c r="A114" s="17">
         <v>4828</v>
       </c>
@@ -21421,7 +21419,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="115" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:47" s="1" customFormat="1">
       <c r="A115" s="17">
         <v>4638</v>
       </c>
@@ -21564,7 +21562,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="116" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:47" s="1" customFormat="1">
       <c r="A116" s="17">
         <v>5191</v>
       </c>
@@ -21707,7 +21705,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="117" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:47" s="1" customFormat="1">
       <c r="A117" s="17">
         <v>5189</v>
       </c>
@@ -21850,7 +21848,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="118" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:47" s="1" customFormat="1">
       <c r="A118" s="17">
         <v>5169</v>
       </c>
@@ -21993,7 +21991,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="119" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:47" s="1" customFormat="1">
       <c r="A119" s="17">
         <v>5075</v>
       </c>
@@ -22136,7 +22134,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="120" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:47" s="1" customFormat="1">
       <c r="A120" s="17">
         <v>5283</v>
       </c>
@@ -22279,7 +22277,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="121" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:47" s="1" customFormat="1">
       <c r="A121" s="17">
         <v>5779</v>
       </c>
@@ -22422,7 +22420,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="122" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:47" s="1" customFormat="1">
       <c r="A122" s="17">
         <v>5505</v>
       </c>
@@ -22565,7 +22563,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="123" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:47" s="1" customFormat="1">
       <c r="A123" s="17">
         <v>4592</v>
       </c>
@@ -22708,7 +22706,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="124" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:47" s="1" customFormat="1">
       <c r="A124" s="17">
         <v>5346</v>
       </c>
@@ -22851,7 +22849,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="125" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:47" s="1" customFormat="1">
       <c r="A125" s="17">
         <v>4875</v>
       </c>
@@ -22994,7 +22992,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="126" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:47" s="1" customFormat="1">
       <c r="A126" s="17">
         <v>5559</v>
       </c>
@@ -23137,7 +23135,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="127" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:47" s="1" customFormat="1">
       <c r="A127" s="17">
         <v>5711</v>
       </c>
@@ -23280,7 +23278,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="128" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:47" s="1" customFormat="1">
       <c r="A128" s="17">
         <v>4826</v>
       </c>
@@ -23423,7 +23421,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="129" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:47" s="1" customFormat="1">
       <c r="A129" s="17">
         <v>5392</v>
       </c>
@@ -23566,7 +23564,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="130" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:47" s="1" customFormat="1">
       <c r="A130" s="17">
         <v>4829</v>
       </c>
@@ -23709,7 +23707,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="131" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:47" s="1" customFormat="1">
       <c r="A131" s="17">
         <v>5782</v>
       </c>
@@ -23852,7 +23850,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="132" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:47" s="1" customFormat="1">
       <c r="A132" s="17">
         <v>5408</v>
       </c>
@@ -23995,7 +23993,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="133" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:47" s="1" customFormat="1">
       <c r="A133" s="17">
         <v>5330</v>
       </c>
@@ -24138,7 +24136,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="134" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:47" s="6" customFormat="1">
       <c r="A134" s="16">
         <v>6219</v>
       </c>
@@ -24281,7 +24279,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="135" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:47" s="6" customFormat="1">
       <c r="A135" s="16">
         <v>6128</v>
       </c>
@@ -24424,7 +24422,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="136" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:47" s="6" customFormat="1">
       <c r="A136" s="16">
         <v>6205</v>
       </c>
@@ -24567,7 +24565,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="137" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:47" s="6" customFormat="1">
       <c r="A137" s="16">
         <v>6097</v>
       </c>
@@ -24710,7 +24708,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="138" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:47" s="6" customFormat="1">
       <c r="A138" s="16">
         <v>6135</v>
       </c>
@@ -24853,7 +24851,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="139" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:47" s="6" customFormat="1">
       <c r="A139" s="16">
         <v>6174</v>
       </c>
@@ -24996,7 +24994,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="140" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:47" s="6" customFormat="1">
       <c r="A140" s="16">
         <v>6096</v>
       </c>
@@ -25139,7 +25137,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="141" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:47" s="6" customFormat="1">
       <c r="A141" s="16">
         <v>6138</v>
       </c>
@@ -25282,7 +25280,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="142" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:47" s="6" customFormat="1">
       <c r="A142" s="16">
         <v>6044</v>
       </c>
@@ -25425,7 +25423,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="143" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:47" s="6" customFormat="1">
       <c r="A143" s="16">
         <v>5939</v>
       </c>
@@ -25568,7 +25566,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="144" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:47" s="6" customFormat="1">
       <c r="A144" s="16">
         <v>6000</v>
       </c>
@@ -25711,7 +25709,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="145" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:47" s="6" customFormat="1">
       <c r="A145" s="16">
         <v>6043</v>
       </c>
@@ -25854,7 +25852,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="146" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:47" s="6" customFormat="1">
       <c r="A146" s="16">
         <v>6105</v>
       </c>
@@ -25997,7 +25995,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="147" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:47" s="6" customFormat="1">
       <c r="A147" s="16">
         <v>5850</v>
       </c>
@@ -26140,7 +26138,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="148" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:47" s="6" customFormat="1">
       <c r="A148" s="16">
         <v>5833</v>
       </c>
@@ -26283,7 +26281,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="149" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:47" s="6" customFormat="1">
       <c r="A149" s="16">
         <v>5855</v>
       </c>
@@ -26426,7 +26424,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="150" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:47" s="6" customFormat="1">
       <c r="A150" s="16">
         <v>6161</v>
       </c>
@@ -26569,7 +26567,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="151" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:47" s="6" customFormat="1">
       <c r="A151" s="16">
         <v>6074</v>
       </c>
@@ -26712,7 +26710,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="152" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:47" s="6" customFormat="1">
       <c r="A152" s="16">
         <v>6072</v>
       </c>
@@ -26855,7 +26853,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="153" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:47" s="6" customFormat="1">
       <c r="A153" s="16">
         <v>6209</v>
       </c>
@@ -26998,7 +26996,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="154" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:47" s="6" customFormat="1">
       <c r="A154" s="16">
         <v>6104</v>
       </c>
@@ -27141,7 +27139,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="155" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:47" s="2" customFormat="1">
       <c r="A155" s="17">
         <v>6323</v>
       </c>
@@ -27284,7 +27282,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="156" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:47" s="2" customFormat="1">
       <c r="A156" s="17">
         <v>6322</v>
       </c>
@@ -27427,7 +27425,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="157" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:47" s="2" customFormat="1">
       <c r="A157" s="17">
         <v>6492</v>
       </c>
@@ -27570,7 +27568,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="158" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:47" s="2" customFormat="1">
       <c r="A158" s="17">
         <v>6346</v>
       </c>
@@ -27713,7 +27711,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="159" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:47" s="2" customFormat="1">
       <c r="A159" s="17">
         <v>6399</v>
       </c>
@@ -27856,7 +27854,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="160" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:47" s="2" customFormat="1">
       <c r="A160" s="17">
         <v>6295</v>
       </c>
@@ -27999,7 +27997,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="161" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:47" s="2" customFormat="1">
       <c r="A161" s="17">
         <v>6405</v>
       </c>
@@ -28154,48 +28152,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7434C2A8-4D4F-CE46-B476-FC058505342A}">
   <dimension ref="A1:AU221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC185" workbookViewId="0">
-      <selection activeCell="AU208" sqref="AU208"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A221"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="18"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" customWidth="1"/>
-    <col min="18" max="18" width="24.140625" customWidth="1"/>
-    <col min="19" max="19" width="23" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" customWidth="1"/>
-    <col min="25" max="26" width="11.7109375" customWidth="1"/>
-    <col min="28" max="28" width="15" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" customWidth="1"/>
-    <col min="31" max="31" width="13.140625" customWidth="1"/>
-    <col min="32" max="32" width="20" customWidth="1"/>
-    <col min="36" max="36" width="10.85546875" customWidth="1"/>
-    <col min="37" max="37" width="14.5703125" customWidth="1"/>
-    <col min="38" max="38" width="17" customWidth="1"/>
-    <col min="39" max="39" width="13.42578125" customWidth="1"/>
-    <col min="40" max="40" width="12.42578125" customWidth="1"/>
-    <col min="41" max="41" width="17.28515625" customWidth="1"/>
-    <col min="42" max="42" width="13.5703125" customWidth="1"/>
-    <col min="43" max="43" width="16.5703125" customWidth="1"/>
-    <col min="44" max="44" width="11.7109375" customWidth="1"/>
-    <col min="45" max="45" width="14.42578125" customWidth="1"/>
-    <col min="46" max="46" width="15.85546875" customWidth="1"/>
-    <col min="47" max="47" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.9140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.08203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.58203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.9140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.9140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.4140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.4140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="87.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.4140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="45.58203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.58203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.9140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -28338,7 +28350,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47">
       <c r="A2" s="3">
         <v>1236</v>
       </c>
@@ -28481,7 +28493,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47">
       <c r="A3" s="3">
         <v>1987</v>
       </c>
@@ -28624,7 +28636,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47">
       <c r="A4" s="3">
         <v>1979</v>
       </c>
@@ -28767,7 +28779,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47">
       <c r="A5" s="3">
         <v>871</v>
       </c>
@@ -28910,7 +28922,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47">
       <c r="A6" s="3">
         <v>3665</v>
       </c>
@@ -29053,7 +29065,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47">
       <c r="A7" s="3">
         <v>3312</v>
       </c>
@@ -29196,7 +29208,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47">
       <c r="A8" s="3">
         <v>1437</v>
       </c>
@@ -29339,7 +29351,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47">
       <c r="A9" s="3">
         <v>1455</v>
       </c>
@@ -29482,7 +29494,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47">
       <c r="A10" s="3">
         <v>53</v>
       </c>
@@ -29625,7 +29637,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47">
       <c r="A11" s="3">
         <v>3073</v>
       </c>
@@ -29768,7 +29780,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47">
       <c r="A12" s="3">
         <v>2002</v>
       </c>
@@ -29911,7 +29923,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47">
       <c r="A13" s="3">
         <v>1903</v>
       </c>
@@ -30054,7 +30066,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47">
       <c r="A14" s="3">
         <v>1540</v>
       </c>
@@ -30197,7 +30209,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47">
       <c r="A15" s="3">
         <v>1354</v>
       </c>
@@ -30340,7 +30352,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47">
       <c r="A16" s="3">
         <v>1424</v>
       </c>
@@ -30483,7 +30495,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47">
       <c r="A17" s="3">
         <v>2214</v>
       </c>
@@ -30626,7 +30638,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47">
       <c r="A18" s="3">
         <v>3537</v>
       </c>
@@ -30769,7 +30781,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47">
       <c r="A19" s="3">
         <v>1598</v>
       </c>
@@ -30912,7 +30924,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47">
       <c r="A20" s="3">
         <v>3235</v>
       </c>
@@ -31055,7 +31067,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47">
       <c r="A21" s="3">
         <v>1958</v>
       </c>
@@ -31198,7 +31210,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47">
       <c r="A22" s="3">
         <v>1298</v>
       </c>
@@ -31341,7 +31353,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47">
       <c r="A23" s="3">
         <v>1487</v>
       </c>
@@ -31484,7 +31496,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47">
       <c r="A24" s="3">
         <v>2069</v>
       </c>
@@ -31627,7 +31639,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47">
       <c r="A25" s="3">
         <v>1360</v>
       </c>
@@ -31770,7 +31782,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" s="7" customFormat="1">
       <c r="A26" s="18">
         <v>3351</v>
       </c>
@@ -31913,7 +31925,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" s="7" customFormat="1">
       <c r="A27" s="18">
         <v>876</v>
       </c>
@@ -32056,7 +32068,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" s="7" customFormat="1">
       <c r="A28" s="18">
         <v>2748</v>
       </c>
@@ -32199,7 +32211,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" s="7" customFormat="1">
       <c r="A29" s="18">
         <v>2737</v>
       </c>
@@ -32342,7 +32354,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" s="7" customFormat="1">
       <c r="A30" s="18">
         <v>2765</v>
       </c>
@@ -32485,7 +32497,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" s="7" customFormat="1">
       <c r="A31" s="18">
         <v>650</v>
       </c>
@@ -32628,7 +32640,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" s="7" customFormat="1">
       <c r="A32" s="18">
         <v>651</v>
       </c>
@@ -32771,7 +32783,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" s="7" customFormat="1">
       <c r="A33" s="18">
         <v>3846</v>
       </c>
@@ -32914,7 +32926,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" s="7" customFormat="1">
       <c r="A34" s="18">
         <v>3833</v>
       </c>
@@ -33057,7 +33069,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" s="7" customFormat="1">
       <c r="A35" s="18">
         <v>3848</v>
       </c>
@@ -33200,7 +33212,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" s="7" customFormat="1">
       <c r="A36" s="18">
         <v>530</v>
       </c>
@@ -33343,7 +33355,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" s="7" customFormat="1">
       <c r="A37" s="18">
         <v>2587</v>
       </c>
@@ -33486,7 +33498,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" s="7" customFormat="1">
       <c r="A38" s="18">
         <v>2589</v>
       </c>
@@ -33629,7 +33641,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:47" s="7" customFormat="1">
       <c r="A39" s="18">
         <v>2604</v>
       </c>
@@ -33772,7 +33784,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" s="7" customFormat="1">
       <c r="A40" s="18">
         <v>2607</v>
       </c>
@@ -33915,7 +33927,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" s="7" customFormat="1">
       <c r="A41" s="18">
         <v>961</v>
       </c>
@@ -34058,7 +34070,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" s="7" customFormat="1">
       <c r="A42" s="18">
         <v>967</v>
       </c>
@@ -34201,7 +34213,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" s="7" customFormat="1">
       <c r="A43" s="18">
         <v>3211</v>
       </c>
@@ -34344,7 +34356,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" s="7" customFormat="1">
       <c r="A44" s="18">
         <v>4029</v>
       </c>
@@ -34487,7 +34499,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" s="7" customFormat="1">
       <c r="A45" s="18">
         <v>3412</v>
       </c>
@@ -34630,7 +34642,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:47" s="7" customFormat="1">
       <c r="A46" s="18">
         <v>3397</v>
       </c>
@@ -34773,7 +34785,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:47" s="7" customFormat="1">
       <c r="A47" s="18">
         <v>3415</v>
       </c>
@@ -34916,7 +34928,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" s="7" customFormat="1">
       <c r="A48" s="18">
         <v>190</v>
       </c>
@@ -35059,7 +35071,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:47" s="7" customFormat="1">
       <c r="A49" s="18">
         <v>1076</v>
       </c>
@@ -35202,7 +35214,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:47" s="7" customFormat="1">
       <c r="A50" s="18">
         <v>1090</v>
       </c>
@@ -35345,7 +35357,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:47" s="7" customFormat="1">
       <c r="A51" s="18">
         <v>225</v>
       </c>
@@ -35488,7 +35500,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:47" s="7" customFormat="1">
       <c r="A52" s="18">
         <v>227</v>
       </c>
@@ -35631,7 +35643,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:47" s="7" customFormat="1">
       <c r="A53" s="18">
         <v>2541</v>
       </c>
@@ -35774,7 +35786,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:47" s="7" customFormat="1">
       <c r="A54" s="18">
         <v>2246</v>
       </c>
@@ -35917,7 +35929,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:47" s="7" customFormat="1">
       <c r="A55" s="18">
         <v>2249</v>
       </c>
@@ -36060,7 +36072,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:47" s="7" customFormat="1">
       <c r="A56" s="18">
         <v>694</v>
       </c>
@@ -36203,7 +36215,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:47" s="7" customFormat="1">
       <c r="A57" s="18">
         <v>4355</v>
       </c>
@@ -36346,7 +36358,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:47" s="7" customFormat="1">
       <c r="A58" s="18">
         <v>739</v>
       </c>
@@ -36489,7 +36501,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:47" s="7" customFormat="1">
       <c r="A59" s="18">
         <v>2556</v>
       </c>
@@ -36632,7 +36644,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:47" s="7" customFormat="1">
       <c r="A60" s="18">
         <v>3618</v>
       </c>
@@ -36775,7 +36787,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:47" s="7" customFormat="1">
       <c r="A61" s="18">
         <v>3187</v>
       </c>
@@ -36918,7 +36930,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:47" s="7" customFormat="1">
       <c r="A62" s="18">
         <v>3185</v>
       </c>
@@ -37061,7 +37073,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:47" s="7" customFormat="1">
       <c r="A63" s="18">
         <v>2370</v>
       </c>
@@ -37204,7 +37216,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:47" s="7" customFormat="1">
       <c r="A64" s="18">
         <v>2364</v>
       </c>
@@ -37347,7 +37359,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" s="7" customFormat="1">
       <c r="A65" s="18">
         <v>3170</v>
       </c>
@@ -37490,7 +37502,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" s="7" customFormat="1">
       <c r="A66" s="18">
         <v>810</v>
       </c>
@@ -37633,7 +37645,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" s="7" customFormat="1">
       <c r="A67" s="18">
         <v>3814</v>
       </c>
@@ -37776,7 +37788,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" s="7" customFormat="1">
       <c r="A68" s="18">
         <v>3342</v>
       </c>
@@ -37919,7 +37931,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" s="7" customFormat="1">
       <c r="A69" s="18">
         <v>4201</v>
       </c>
@@ -38062,7 +38074,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47">
       <c r="A70" s="3">
         <v>2670</v>
       </c>
@@ -38205,7 +38217,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47">
       <c r="A71" s="3">
         <v>1868</v>
       </c>
@@ -38348,7 +38360,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:47">
       <c r="A72" s="3">
         <v>2971</v>
       </c>
@@ -38491,7 +38503,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:47">
       <c r="A73" s="3">
         <v>3120</v>
       </c>
@@ -38634,7 +38646,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:47">
       <c r="A74" s="3">
         <v>2290</v>
       </c>
@@ -38777,7 +38789,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:47">
       <c r="A75" s="3">
         <v>2694</v>
       </c>
@@ -38920,7 +38932,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:47">
       <c r="A76" s="3">
         <v>1857</v>
       </c>
@@ -39063,7 +39075,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:47">
       <c r="A77" s="3">
         <v>4294</v>
       </c>
@@ -39206,7 +39218,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:47">
       <c r="A78" s="3">
         <v>4330</v>
       </c>
@@ -39349,7 +39361,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:47">
       <c r="A79" s="3">
         <v>2875</v>
       </c>
@@ -39492,7 +39504,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="80" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:47">
       <c r="A80" s="3">
         <v>511</v>
       </c>
@@ -39635,7 +39647,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:47">
       <c r="A81" s="3">
         <v>1842</v>
       </c>
@@ -39778,7 +39790,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="82" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:47">
       <c r="A82" s="3">
         <v>1379</v>
       </c>
@@ -39921,7 +39933,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:47">
       <c r="A83" s="3">
         <v>2331</v>
       </c>
@@ -40064,7 +40076,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:47">
       <c r="A84" s="3">
         <v>4242</v>
       </c>
@@ -40207,7 +40219,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="85" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:47">
       <c r="A85" s="3">
         <v>3122</v>
       </c>
@@ -40350,7 +40362,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="86" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:47">
       <c r="A86" s="3">
         <v>985</v>
       </c>
@@ -40493,7 +40505,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:47">
       <c r="A87" s="3">
         <v>3577</v>
       </c>
@@ -40636,7 +40648,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="88" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:47">
       <c r="A88" s="3">
         <v>4057</v>
       </c>
@@ -40779,7 +40791,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="89" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:47">
       <c r="A89" s="3">
         <v>4297</v>
       </c>
@@ -40922,7 +40934,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="90" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:47">
       <c r="A90" s="3">
         <v>2178</v>
       </c>
@@ -41065,7 +41077,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="91" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:47">
       <c r="A91" s="3">
         <v>162</v>
       </c>
@@ -41208,7 +41220,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:47">
       <c r="A92" s="3">
         <v>982</v>
       </c>
@@ -41351,7 +41363,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="93" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:47">
       <c r="A93" s="3">
         <v>4293</v>
       </c>
@@ -41494,7 +41506,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:47">
       <c r="A94" s="3">
         <v>3141</v>
       </c>
@@ -41637,7 +41649,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="95" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:47">
       <c r="A95" s="3">
         <v>2319</v>
       </c>
@@ -41780,7 +41792,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="96" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:47">
       <c r="A96" s="3">
         <v>3119</v>
       </c>
@@ -41923,7 +41935,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="97" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:47">
       <c r="A97" s="3">
         <v>989</v>
       </c>
@@ -42066,7 +42078,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="98" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:47">
       <c r="A98" s="3">
         <v>387</v>
       </c>
@@ -42209,7 +42221,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="99" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:47">
       <c r="A99" s="3">
         <v>3574</v>
       </c>
@@ -42352,7 +42364,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="100" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:47">
       <c r="A100" s="3">
         <v>2429</v>
       </c>
@@ -42495,7 +42507,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="101" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:47">
       <c r="A101" s="3">
         <v>2698</v>
       </c>
@@ -42638,7 +42650,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="102" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:47">
       <c r="A102" s="3">
         <v>3331</v>
       </c>
@@ -42781,7 +42793,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="103" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:47">
       <c r="A103" s="3">
         <v>1847</v>
       </c>
@@ -42924,7 +42936,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="104" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:47">
       <c r="A104" s="3">
         <v>4160</v>
       </c>
@@ -43067,7 +43079,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="105" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:47">
       <c r="A105" s="3">
         <v>940</v>
       </c>
@@ -43210,7 +43222,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="106" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:47">
       <c r="A106" s="3">
         <v>4045</v>
       </c>
@@ -43353,7 +43365,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="107" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:47">
       <c r="A107" s="3">
         <v>991</v>
       </c>
@@ -43496,7 +43508,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="108" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:47">
       <c r="A108" s="3">
         <v>3135</v>
       </c>
@@ -43639,7 +43651,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="109" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:47">
       <c r="A109" s="3">
         <v>2972</v>
       </c>
@@ -43782,7 +43794,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="110" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:47">
       <c r="A110" s="3">
         <v>786</v>
       </c>
@@ -43925,7 +43937,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="111" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:47">
       <c r="A111" s="3">
         <v>4290</v>
       </c>
@@ -44068,7 +44080,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="112" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:47">
       <c r="A112" s="3">
         <v>2390</v>
       </c>
@@ -44211,7 +44223,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="113" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:47">
       <c r="A113" s="3">
         <v>3130</v>
       </c>
@@ -44354,7 +44366,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="114" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:47">
       <c r="A114" s="3">
         <v>479</v>
       </c>
@@ -44497,7 +44509,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="115" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:47">
       <c r="A115" s="3">
         <v>267</v>
       </c>
@@ -44640,7 +44652,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="116" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:47">
       <c r="A116" s="3">
         <v>462</v>
       </c>
@@ -44783,7 +44795,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="117" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:47">
       <c r="A117" s="3">
         <v>2427</v>
       </c>
@@ -44926,7 +44938,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="118" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:47">
       <c r="A118" s="3">
         <v>3441</v>
       </c>
@@ -45069,7 +45081,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="119" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:47">
       <c r="A119" s="3">
         <v>2384</v>
       </c>
@@ -45212,7 +45224,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="120" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:47">
       <c r="A120" s="3">
         <v>1391</v>
       </c>
@@ -45355,7 +45367,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="121" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:47">
       <c r="A121" s="3">
         <v>2644</v>
       </c>
@@ -45498,7 +45510,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="122" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:47">
       <c r="A122" s="3">
         <v>151</v>
       </c>
@@ -45641,7 +45653,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="123" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:47">
       <c r="A123" s="3">
         <v>2235</v>
       </c>
@@ -45784,7 +45796,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="124" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:47">
       <c r="A124" s="3">
         <v>4292</v>
       </c>
@@ -45927,7 +45939,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="125" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:47">
       <c r="A125" s="3">
         <v>2658</v>
       </c>
@@ -46070,7 +46082,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="126" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:47">
       <c r="A126" s="3">
         <v>3429</v>
       </c>
@@ -46213,7 +46225,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="127" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:47">
       <c r="A127" s="3">
         <v>477</v>
       </c>
@@ -46356,7 +46368,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="128" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:47">
       <c r="A128" s="3">
         <v>2433</v>
       </c>
@@ -46499,7 +46511,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="129" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:47">
       <c r="A129" s="3">
         <v>4038</v>
       </c>
@@ -46642,7 +46654,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="130" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:47" s="7" customFormat="1">
       <c r="A130" s="18">
         <v>5707</v>
       </c>
@@ -46785,7 +46797,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="131" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:47" s="7" customFormat="1">
       <c r="A131" s="18">
         <v>5714</v>
       </c>
@@ -46928,7 +46940,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="132" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:47" s="7" customFormat="1">
       <c r="A132" s="18">
         <v>4880</v>
       </c>
@@ -47071,7 +47083,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="133" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:47" s="7" customFormat="1">
       <c r="A133" s="18">
         <v>5410</v>
       </c>
@@ -47214,7 +47226,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="134" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:47" s="7" customFormat="1">
       <c r="A134" s="18">
         <v>4877</v>
       </c>
@@ -47357,7 +47369,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="135" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:47" s="7" customFormat="1">
       <c r="A135" s="18">
         <v>4474</v>
       </c>
@@ -47500,7 +47512,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="136" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:47" s="7" customFormat="1">
       <c r="A136" s="18">
         <v>4702</v>
       </c>
@@ -47643,7 +47655,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="137" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:47" s="7" customFormat="1">
       <c r="A137" s="18">
         <v>5363</v>
       </c>
@@ -47786,7 +47798,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="138" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:47" s="7" customFormat="1">
       <c r="A138" s="18">
         <v>5261</v>
       </c>
@@ -47929,7 +47941,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="139" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:47" s="7" customFormat="1">
       <c r="A139" s="18">
         <v>5039</v>
       </c>
@@ -48072,7 +48084,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="140" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:47" s="7" customFormat="1">
       <c r="A140" s="18">
         <v>5411</v>
       </c>
@@ -48215,7 +48227,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="141" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:47" s="7" customFormat="1">
       <c r="A141" s="18">
         <v>5025</v>
       </c>
@@ -48358,7 +48370,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="142" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:47" s="7" customFormat="1">
       <c r="A142" s="18">
         <v>4597</v>
       </c>
@@ -48501,7 +48513,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="143" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:47" s="7" customFormat="1">
       <c r="A143" s="18">
         <v>5335</v>
       </c>
@@ -48644,7 +48656,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="144" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:47" s="7" customFormat="1">
       <c r="A144" s="18">
         <v>4401</v>
       </c>
@@ -48787,7 +48799,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="145" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:47" s="7" customFormat="1">
       <c r="A145" s="18">
         <v>4827</v>
       </c>
@@ -48930,7 +48942,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="146" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:47" s="7" customFormat="1">
       <c r="A146" s="18">
         <v>4851</v>
       </c>
@@ -49073,7 +49085,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="147" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:47" s="7" customFormat="1">
       <c r="A147" s="18">
         <v>4589</v>
       </c>
@@ -49216,7 +49228,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="148" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:47" s="7" customFormat="1">
       <c r="A148" s="18">
         <v>5317</v>
       </c>
@@ -49359,7 +49371,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="149" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:47" s="7" customFormat="1">
       <c r="A149" s="18">
         <v>5286</v>
       </c>
@@ -49502,7 +49514,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="150" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:47" s="7" customFormat="1">
       <c r="A150" s="18">
         <v>5193</v>
       </c>
@@ -49645,7 +49657,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="151" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:47" s="7" customFormat="1">
       <c r="A151" s="18">
         <v>4565</v>
       </c>
@@ -49788,7 +49800,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="152" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:47" s="7" customFormat="1">
       <c r="A152" s="18">
         <v>4828</v>
       </c>
@@ -49931,7 +49943,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="153" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:47" s="7" customFormat="1">
       <c r="A153" s="18">
         <v>4638</v>
       </c>
@@ -50074,7 +50086,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="154" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:47" s="7" customFormat="1">
       <c r="A154" s="18">
         <v>5191</v>
       </c>
@@ -50217,7 +50229,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="155" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:47" s="7" customFormat="1">
       <c r="A155" s="18">
         <v>5189</v>
       </c>
@@ -50360,7 +50372,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="156" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:47" s="7" customFormat="1">
       <c r="A156" s="18">
         <v>5169</v>
       </c>
@@ -50503,7 +50515,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="157" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:47" s="7" customFormat="1">
       <c r="A157" s="18">
         <v>5075</v>
       </c>
@@ -50646,7 +50658,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="158" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:47" s="7" customFormat="1">
       <c r="A158" s="18">
         <v>5283</v>
       </c>
@@ -50789,7 +50801,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="159" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:47" s="7" customFormat="1">
       <c r="A159" s="18">
         <v>5779</v>
       </c>
@@ -50932,7 +50944,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="160" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:47" s="7" customFormat="1">
       <c r="A160" s="18">
         <v>5505</v>
       </c>
@@ -51075,7 +51087,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="161" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:47" s="7" customFormat="1">
       <c r="A161" s="18">
         <v>5413</v>
       </c>
@@ -51218,7 +51230,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="162" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:47" s="7" customFormat="1">
       <c r="A162" s="18">
         <v>4592</v>
       </c>
@@ -51361,7 +51373,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="163" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:47" s="7" customFormat="1">
       <c r="A163" s="18">
         <v>5346</v>
       </c>
@@ -51504,7 +51516,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="164" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:47" s="7" customFormat="1">
       <c r="A164" s="18">
         <v>4875</v>
       </c>
@@ -51647,7 +51659,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="165" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:47" s="7" customFormat="1">
       <c r="A165" s="18">
         <v>5559</v>
       </c>
@@ -51790,7 +51802,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="166" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:47" s="7" customFormat="1">
       <c r="A166" s="18">
         <v>5711</v>
       </c>
@@ -51933,7 +51945,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="167" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:47" s="7" customFormat="1">
       <c r="A167" s="18">
         <v>4826</v>
       </c>
@@ -52076,7 +52088,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="168" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:47" s="7" customFormat="1">
       <c r="A168" s="18">
         <v>5392</v>
       </c>
@@ -52219,7 +52231,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="169" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:47" s="7" customFormat="1">
       <c r="A169" s="18">
         <v>4829</v>
       </c>
@@ -52362,7 +52374,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="170" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:47" s="7" customFormat="1">
       <c r="A170" s="18">
         <v>5333</v>
       </c>
@@ -52505,7 +52517,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="171" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:47" s="7" customFormat="1">
       <c r="A171" s="18">
         <v>5782</v>
       </c>
@@ -52648,7 +52660,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="172" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:47" s="7" customFormat="1">
       <c r="A172" s="18">
         <v>5409</v>
       </c>
@@ -52791,7 +52803,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="173" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:47" s="7" customFormat="1">
       <c r="A173" s="18">
         <v>5408</v>
       </c>
@@ -52934,7 +52946,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="174" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:47" s="7" customFormat="1">
       <c r="A174" s="18">
         <v>5330</v>
       </c>
@@ -53077,7 +53089,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="175" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:47" s="7" customFormat="1">
       <c r="A175" s="18">
         <v>4594</v>
       </c>
@@ -53220,7 +53232,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="176" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:47" s="7" customFormat="1">
       <c r="A176" s="18">
         <v>4696</v>
       </c>
@@ -53363,7 +53375,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="177" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:47" s="7" customFormat="1">
       <c r="A177" s="18">
         <v>5389</v>
       </c>
@@ -53506,7 +53518,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="178" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:47" s="7" customFormat="1">
       <c r="A178" s="18">
         <v>5534</v>
       </c>
@@ -53649,7 +53661,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="179" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:47" s="7" customFormat="1">
       <c r="A179" s="18">
         <v>5589</v>
       </c>
@@ -53792,7 +53804,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="180" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:47" s="7" customFormat="1">
       <c r="A180" s="18">
         <v>4853</v>
       </c>
@@ -53935,7 +53947,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="181" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:47" s="7" customFormat="1">
       <c r="A181" s="18">
         <v>5407</v>
       </c>
@@ -54078,7 +54090,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="182" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:47" s="7" customFormat="1">
       <c r="A182" s="18">
         <v>5125</v>
       </c>
@@ -54221,7 +54233,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="183" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:47" s="7" customFormat="1">
       <c r="A183" s="18">
         <v>4904</v>
       </c>
@@ -54364,7 +54376,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="184" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:47" s="7" customFormat="1">
       <c r="A184" s="18">
         <v>5347</v>
       </c>
@@ -54507,7 +54519,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="185" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:47" s="10" customFormat="1">
       <c r="A185" s="19">
         <v>6089</v>
       </c>
@@ -54610,7 +54622,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="186" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:47">
       <c r="A186" s="11">
         <v>6097</v>
       </c>
@@ -54711,7 +54723,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="187" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:47" s="10" customFormat="1">
       <c r="A187" s="19">
         <v>6018</v>
       </c>
@@ -54814,7 +54826,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="188" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:47">
       <c r="A188" s="11">
         <v>6135</v>
       </c>
@@ -54915,7 +54927,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="189" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:47">
       <c r="A189" s="11">
         <v>6174</v>
       </c>
@@ -55018,7 +55030,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="190" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:47">
       <c r="A190" s="11">
         <v>6096</v>
       </c>
@@ -55119,7 +55131,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="191" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:47">
       <c r="A191" s="11">
         <v>6138</v>
       </c>
@@ -55220,7 +55232,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="192" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:47" s="10" customFormat="1">
       <c r="A192" s="19">
         <v>6219</v>
       </c>
@@ -55321,7 +55333,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="193" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:47" s="10" customFormat="1">
       <c r="A193" s="19">
         <v>6128</v>
       </c>
@@ -55422,7 +55434,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="194" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:47">
       <c r="A194" s="11">
         <v>5939</v>
       </c>
@@ -55525,7 +55537,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="195" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:47">
       <c r="A195" s="11">
         <v>6000</v>
       </c>
@@ -55626,7 +55638,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="196" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:47">
       <c r="A196" s="11">
         <v>6043</v>
       </c>
@@ -55727,7 +55739,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="197" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:47">
       <c r="A197" s="11">
         <v>6105</v>
       </c>
@@ -55830,7 +55842,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="198" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:47">
       <c r="A198" s="11">
         <v>5833</v>
       </c>
@@ -55935,7 +55947,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="199" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:47" s="10" customFormat="1">
       <c r="A199" s="19">
         <v>6205</v>
       </c>
@@ -56038,7 +56050,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="200" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:47" s="10" customFormat="1">
       <c r="A200" s="19">
         <v>6022</v>
       </c>
@@ -56143,7 +56155,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="201" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:47">
       <c r="A201" s="11">
         <v>5855</v>
       </c>
@@ -56244,7 +56256,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="202" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:47">
       <c r="A202" s="11">
         <v>6161</v>
       </c>
@@ -56347,7 +56359,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="203" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:47">
       <c r="A203" s="11">
         <v>6074</v>
       </c>
@@ -56452,7 +56464,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="204" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:47">
       <c r="A204" s="11">
         <v>6072</v>
       </c>
@@ -56557,7 +56569,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="205" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:47">
       <c r="A205" s="11">
         <v>6209</v>
       </c>
@@ -56662,7 +56674,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="206" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:47">
       <c r="A206" s="11">
         <v>6104</v>
       </c>
@@ -56765,7 +56777,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="207" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:47">
       <c r="A207" s="11">
         <v>5843</v>
       </c>
@@ -56866,7 +56878,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="208" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:47" s="10" customFormat="1">
       <c r="A208" s="19">
         <v>6023</v>
       </c>
@@ -56971,7 +56983,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="209" spans="1:47" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:47" s="10" customFormat="1">
       <c r="A209" s="19">
         <v>5993</v>
       </c>
@@ -57070,7 +57082,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="210" spans="1:47" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:47" s="9" customFormat="1">
       <c r="A210" s="8">
         <v>6342</v>
       </c>
@@ -57213,7 +57225,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="211" spans="1:47" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:47" s="9" customFormat="1">
       <c r="A211" s="8">
         <v>6323</v>
       </c>
@@ -57356,7 +57368,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="212" spans="1:47" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:47" s="9" customFormat="1">
       <c r="A212" s="8">
         <v>6322</v>
       </c>
@@ -57499,7 +57511,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="213" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:47" s="7" customFormat="1">
       <c r="A213" s="18">
         <v>6492</v>
       </c>
@@ -57642,7 +57654,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="214" spans="1:47" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:47" s="9" customFormat="1">
       <c r="A214" s="8">
         <v>6346</v>
       </c>
@@ -57785,7 +57797,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="215" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:47" s="7" customFormat="1">
       <c r="A215" s="18">
         <v>6399</v>
       </c>
@@ -57928,7 +57940,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="216" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:47" s="7" customFormat="1">
       <c r="A216" s="18">
         <v>6306</v>
       </c>
@@ -58071,7 +58083,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="217" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:47" s="7" customFormat="1">
       <c r="A217" s="18">
         <v>6461</v>
       </c>
@@ -58214,7 +58226,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="218" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:47" s="7" customFormat="1">
       <c r="A218" s="18">
         <v>6295</v>
       </c>
@@ -58357,7 +58369,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="219" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:47" s="7" customFormat="1">
       <c r="A219" s="18">
         <v>6405</v>
       </c>
@@ -58500,7 +58512,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="220" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:47" s="7" customFormat="1">
       <c r="A220" s="18">
         <v>6468</v>
       </c>
@@ -58643,7 +58655,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="221" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:47" s="7" customFormat="1">
       <c r="A221" s="18">
         <v>6491</v>
       </c>

</xml_diff>